<commit_message>
Fix bug where warning and errors msgs are printed by mistake
</commit_message>
<xml_diff>
--- a/src/tests/ScriptTest1_Fixes.xlsx
+++ b/src/tests/ScriptTest1_Fixes.xlsx
@@ -556,7 +556,7 @@
   <dimension ref="A1:N574"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -625,21 +625,24 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="14" t="n">
+        <f aca="false">IF(NOT(ISBLANK(C2)),(C2-$N$2)/30, "")</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D2" s="14" t="str">
-        <f aca="false">IF(NOT(ISBLANK(C2)),(C2-$N$2)/30, "")</f>
-        <v/>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="F2" s="1" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G2" s="15" t="n">
         <f aca="false">IF(NOT(ISBLANK(F2)),(F2-$N$2)/30, "")</f>
-        <v>0</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="J2" s="16"/>
       <c r="L2" s="0"/>
@@ -656,21 +659,24 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="D3" s="14" t="str">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="D3" s="14" t="n">
         <f aca="false">IF(NOT(ISBLANK(C3)),(C3-$N$2)/30, "")</f>
-        <v/>
+        <v>0.633333333333333</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G3" s="15" t="n">
         <f aca="false">IF(NOT(ISBLANK(F3)),(F3-$N$2)/30, "")</f>
-        <v>1</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="J3" s="16"/>
       <c r="L3" s="0"/>
@@ -682,21 +688,24 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>411</v>
-      </c>
-      <c r="D4" s="14" t="str">
+        <v>100</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="D4" s="14" t="n">
         <f aca="false">IF(NOT(ISBLANK(C4)),(C4-$N$2)/30, "")</f>
-        <v/>
+        <v>0.8</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G4" s="15" t="n">
         <f aca="false">IF(NOT(ISBLANK(F4)),(F4-$N$2)/30, "")</f>
-        <v>1.03333333333333</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="J4" s="16"/>
     </row>
@@ -706,21 +715,24 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="D5" s="14" t="str">
+        <v>200</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="D5" s="14" t="n">
         <f aca="false">IF(NOT(ISBLANK(C5)),(C5-$N$2)/30, "")</f>
-        <v/>
+        <v>0.966666666666667</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>411</v>
+        <v>4</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="15" t="n">
         <f aca="false">IF(NOT(ISBLANK(F5)),(F5-$N$2)/30, "")</f>
-        <v>1.03333333333333</v>
+        <v>1</v>
       </c>
       <c r="J5" s="16"/>
     </row>
@@ -729,22 +741,13 @@
         <f aca="false">A5+1</f>
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>411</v>
-      </c>
       <c r="D6" s="14" t="str">
         <f aca="false">IF(NOT(ISBLANK(C6)),(C6-$N$2)/30, "")</f>
         <v/>
       </c>
-      <c r="E6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="G6" s="15" t="n">
+      <c r="G6" s="15" t="str">
         <f aca="false">IF(NOT(ISBLANK(F6)),(F6-$N$2)/30, "")</f>
-        <v>1.06666666666667</v>
+        <v/>
       </c>
       <c r="J6" s="16"/>
     </row>
@@ -753,22 +756,13 @@
         <f aca="false">A6+1</f>
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="n">
-        <v>11</v>
-      </c>
       <c r="D7" s="14" t="str">
         <f aca="false">IF(NOT(ISBLANK(C7)),(C7-$N$2)/30, "")</f>
         <v/>
       </c>
-      <c r="E7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="G7" s="15" t="n">
+      <c r="G7" s="15" t="str">
         <f aca="false">IF(NOT(ISBLANK(F7)),(F7-$N$2)/30, "")</f>
-        <v>0.166666666666667</v>
+        <v/>
       </c>
       <c r="J7" s="16"/>
     </row>
@@ -777,22 +771,13 @@
         <f aca="false">A7+1</f>
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="n">
-        <v>42</v>
-      </c>
       <c r="D8" s="14" t="str">
         <f aca="false">IF(NOT(ISBLANK(C8)),(C8-$N$2)/30, "")</f>
         <v/>
       </c>
-      <c r="E8" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="G8" s="15" t="n">
+      <c r="G8" s="15" t="str">
         <f aca="false">IF(NOT(ISBLANK(F8)),(F8-$N$2)/30, "")</f>
-        <v>1.1</v>
+        <v/>
       </c>
       <c r="J8" s="16"/>
     </row>
@@ -801,22 +786,13 @@
         <f aca="false">A8+1</f>
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="n">
-        <v>88</v>
-      </c>
       <c r="D9" s="14" t="str">
         <f aca="false">IF(NOT(ISBLANK(C9)),(C9-$N$2)/30, "")</f>
         <v/>
       </c>
-      <c r="E9" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="G9" s="15" t="n">
+      <c r="G9" s="15" t="str">
         <f aca="false">IF(NOT(ISBLANK(F9)),(F9-$N$2)/30, "")</f>
-        <v>2.33333333333333</v>
+        <v/>
       </c>
       <c r="J9" s="16"/>
     </row>
@@ -825,22 +801,13 @@
         <f aca="false">A9+1</f>
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="n">
-        <v>888</v>
-      </c>
       <c r="D10" s="14" t="str">
         <f aca="false">IF(NOT(ISBLANK(C10)),(C10-$N$2)/30, "")</f>
         <v/>
       </c>
-      <c r="E10" s="1" t="n">
-        <v>88</v>
-      </c>
-      <c r="F10" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="G10" s="15" t="n">
+      <c r="G10" s="15" t="str">
         <f aca="false">IF(NOT(ISBLANK(F10)),(F10-$N$2)/30, "")</f>
-        <v>2.5</v>
+        <v/>
       </c>
       <c r="J10" s="16"/>
     </row>

</xml_diff>